<commit_message>
User Story 02 and Excel Sheet
</commit_message>
<xml_diff>
--- a/Team_DhruvalKunjNihirVyomYash_Report.xlsx
+++ b/Team_DhruvalKunjNihirVyomYash_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunj/Desktop/Stevens/CS555_Final_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79B43C6-19D4-A543-8900-72502DCC6E8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632ED442-D011-3D4D-BD4E-7D60DD466E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15760" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -712,22 +712,22 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>0.5 hour</t>
-  </si>
-  <si>
-    <t>0.75 hour</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>GenerateOutput</t>
   </si>
   <si>
-    <t>us02_birth_b4_date()</t>
-  </si>
-  <si>
-    <t>299-335</t>
+    <t>us02_birth_b4_marriage</t>
+  </si>
+  <si>
+    <t>31-77</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>2 hours</t>
   </si>
 </sst>
 </file>
@@ -2056,7 +2056,7 @@
     <col min="2" max="2" width="6.5" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="45.33203125" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -2614,7 +2614,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2629,7 +2629,7 @@
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
     <col min="15" max="15" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
@@ -2698,28 +2698,28 @@
         <v>211</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G2">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="G2">
-        <v>36</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="K2" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="L2" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="M2" s="18" t="s">
         <v>215</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>217</v>
       </c>
       <c r="O2" s="18"/>
       <c r="P2" s="18"/>

</xml_diff>

<commit_message>
User story 6 added.
</commit_message>
<xml_diff>
--- a/Team_DhruvalKunjNihirVyomYash_Report.xlsx
+++ b/Team_DhruvalKunjNihirVyomYash_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunj/Desktop/Stevens/CS555_Final_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6BE061-09AB-0049-9918-CDEB50A3DFCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712FF5F0-AAC6-6745-84CC-E550BFB911FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="222">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -724,6 +724,18 @@
   </si>
   <si>
     <t>List Upcoming birthdays</t>
+  </si>
+  <si>
+    <t>us06_divorce_b4_death()</t>
+  </si>
+  <si>
+    <t>test_us06_divorce_b4_death()</t>
+  </si>
+  <si>
+    <t>38-44</t>
+  </si>
+  <si>
+    <t>130-172</t>
   </si>
 </sst>
 </file>
@@ -1159,6 +1171,9 @@
                 <c:pt idx="0">
                   <c:v>42409</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>42430</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1170,6 +1185,9 @@
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2204,7 +2222,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2233,105 +2251,99 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E3" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>204</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
         <v>184</v>
@@ -2339,44 +2351,50 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>147</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="D9" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C10" t="s">
-        <v>68</v>
+        <v>109</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+        <v>178</v>
+      </c>
+      <c r="E10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" t="s">
-        <v>151</v>
+        <v>111</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>192</v>
+        <v>178</v>
+      </c>
+      <c r="E11" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -2392,6 +2410,9 @@
       <c r="D12" t="s">
         <v>178</v>
       </c>
+      <c r="E12" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
@@ -2409,86 +2430,86 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="C15" t="s">
-        <v>217</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="C17" t="s">
-        <v>164</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
@@ -2496,13 +2517,13 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C20" t="s">
-        <v>171</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
@@ -2510,13 +2531,13 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>164</v>
       </c>
       <c r="D21" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
@@ -2524,13 +2545,13 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -2538,97 +2559,97 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D24" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="D25" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>204</v>
       </c>
       <c r="D27" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>217</v>
       </c>
       <c r="D29" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
@@ -2636,13 +2657,13 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
@@ -2650,13 +2671,13 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
@@ -2664,13 +2685,13 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
       <c r="D32" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
@@ -2678,97 +2699,97 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D33" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C34" t="s">
-        <v>150</v>
+        <v>68</v>
       </c>
       <c r="D34" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="D35" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="C36" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="D36" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="C37" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="D37" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C38" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D39" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
@@ -2800,6 +2821,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E41">
+    <sortCondition ref="D1"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{F7A48ADE-6A77-304F-ACF8-66038C36A23F}">
@@ -2968,7 +2992,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3013,6 +3037,12 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="2">
+        <v>42430</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
       <c r="F3" s="9" t="e">
         <f>(D3-D2)/E3*60</f>
         <v>#DIV/0!</v>
@@ -3396,8 +3426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3415,7 +3445,7 @@
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
     <col min="15" max="15" width="19.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.1640625" style="17" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3476,13 +3506,42 @@
       <c r="C2" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="18"/>
+      <c r="D2" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2">
+        <v>45</v>
+      </c>
+      <c r="F2" s="21">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>42</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="4"/>
@@ -3927,7 +3986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C20"/>
     </sheetView>
   </sheetViews>
@@ -4162,8 +4221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4257,6 +4316,9 @@
       <c r="C7" s="12" t="s">
         <v>36</v>
       </c>
+      <c r="D7" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Updating files with formating.
</commit_message>
<xml_diff>
--- a/Team_DhruvalKunjNihirVyomYash_Report.xlsx
+++ b/Team_DhruvalKunjNihirVyomYash_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunj/Desktop/Stevens/CS555_Final_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7BD0C1-B626-2B4A-B57C-CFF93D730153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980DBF95-020A-A549-9DAA-CFBCA681CE60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15720" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -744,10 +744,10 @@
     <t>88-121</t>
   </si>
   <si>
-    <t>177-223</t>
-  </si>
-  <si>
     <t>48-54</t>
+  </si>
+  <si>
+    <t>174-220</t>
   </si>
 </sst>
 </file>
@@ -3454,8 +3454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3559,7 +3559,7 @@
         <v>216</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O2" s="18" t="s">
         <v>210</v>
@@ -3568,7 +3568,7 @@
         <v>217</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
User 10 added and completed
</commit_message>
<xml_diff>
--- a/Team_DhruvalKunjNihirVyomYash_Report.xlsx
+++ b/Team_DhruvalKunjNihirVyomYash_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunj/Desktop/Stevens/CS555_Final_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980DBF95-020A-A549-9DAA-CFBCA681CE60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30D1501-0C03-9B49-8776-ACC43043266B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15720" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15720" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="230">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -738,16 +738,28 @@
     <t>Spending time on writing code and reusing the code</t>
   </si>
   <si>
-    <t>32-78</t>
-  </si>
-  <si>
-    <t>88-121</t>
-  </si>
-  <si>
     <t>48-54</t>
   </si>
   <si>
     <t>174-220</t>
+  </si>
+  <si>
+    <t>us10_marriage_after_14()</t>
+  </si>
+  <si>
+    <t>231-277</t>
+  </si>
+  <si>
+    <t>test_us10_marriage_after_14()</t>
+  </si>
+  <si>
+    <t>57-63</t>
+  </si>
+  <si>
+    <t>33-79</t>
+  </si>
+  <si>
+    <t>89-122</t>
   </si>
 </sst>
 </file>
@@ -2238,7 +2250,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2448,6 +2460,9 @@
       </c>
       <c r="D13" t="s">
         <v>178</v>
+      </c>
+      <c r="E13" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -3088,7 +3103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="105" zoomScaleNormal="157" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="105" zoomScaleNormal="157" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -3194,7 +3209,7 @@
         <v>208</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="O2" s="18" t="s">
         <v>210</v>
@@ -3253,7 +3268,7 @@
         <v>209</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="O4" s="17" t="s">
         <v>210</v>
@@ -3454,8 +3469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="C1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3559,7 +3574,7 @@
         <v>216</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="O2" s="18" t="s">
         <v>210</v>
@@ -3568,7 +3583,7 @@
         <v>217</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
@@ -3592,11 +3607,42 @@
       <c r="C4" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
+      <c r="D4" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+      <c r="G4">
+        <v>46</v>
+      </c>
+      <c r="H4" s="21">
+        <v>45</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
@@ -4273,7 +4319,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4591,7 +4637,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>134</v>
       </c>

</xml_diff>